<commit_message>
adding params to 2DOF arm model
</commit_message>
<xml_diff>
--- a/MPC/resources/tone/paramsFits.xlsx
+++ b/MPC/resources/tone/paramsFits.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>MAS</t>
   </si>
@@ -58,6 +58,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Helvetica"/>
+        <family val="2"/>
       </rPr>
       <t>: Threshold data from Powers (1988). Stiffness &amp; damping data from McCrea (2003).</t>
     </r>
@@ -67,13 +68,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -91,6 +98,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,19 +139,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -205,25 +242,28 @@
                     <a:alpha val="80000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:prstDash val="sysDash"/>
+                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:backward val="2.0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.125758967629046"/>
-                  <c:y val="-0.447230242053077"/>
+                  <c:x val="-0.0499304461942257"/>
+                  <c:y val="-0.279614319043453"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
-                  <a:noFill/>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -361,13 +401,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="564067728"/>
-        <c:axId val="564071248"/>
+        <c:axId val="161215136"/>
+        <c:axId val="154151536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="564067728"/>
+        <c:axId val="161215136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -385,6 +426,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MAS Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -421,12 +518,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="564071248"/>
+        <c:crossAx val="154151536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="564071248"/>
+        <c:axId val="154151536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,6 +543,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Angular</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Threshold [deg]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -483,7 +641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="564067728"/>
+        <c:crossAx val="161215136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -495,6 +653,785 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>stiffness [N-m/deg-kg]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="31750" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.103434820647419"/>
+                  <c:y val="-0.053280475357247"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.000155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000207</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000264</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000233</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.000303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.000413</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00043</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.000509</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.000658</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.000461</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.000549</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.000671</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.000842</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.001232</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>damping [N-m-s/deg-kg]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="31750" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:alpha val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0841207349081365"/>
+                  <c:y val="-0.114968649752114"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$21:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2.01E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.67E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.72E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.37E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.37E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.26E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.53E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0001265</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0001725</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.000183</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0002263</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.37E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.000162</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0003708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0002749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="220243936"/>
+        <c:axId val="219270368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="220243936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MAS</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Score</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219270368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="219270368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Viscoelastic Parameter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="220243936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -572,6 +1509,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1088,17 +2065,533 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1115,6 +2608,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1386,38 +2909,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1428,10 +2943,8 @@
         <f t="shared" ref="C2:C15" si="0" xml:space="preserve"> B2*180/3.14</f>
         <v>14.904458598726116</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1442,10 +2955,8 @@
         <f t="shared" si="0"/>
         <v>34.968152866242036</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1456,10 +2967,8 @@
         <f t="shared" si="0"/>
         <v>57.324840764331206</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1470,10 +2979,8 @@
         <f t="shared" si="0"/>
         <v>57.324840764331206</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1.5</v>
       </c>
@@ -1484,10 +2991,8 @@
         <f t="shared" si="0"/>
         <v>25.796178343949045</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1498,10 +3003,8 @@
         <f t="shared" si="0"/>
         <v>24.076433121019104</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1512,10 +3015,8 @@
         <f t="shared" si="0"/>
         <v>13.757961783439489</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1526,10 +3027,8 @@
         <f t="shared" si="0"/>
         <v>22.356687898089174</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1540,10 +3039,8 @@
         <f t="shared" si="0"/>
         <v>26.942675159235666</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1554,10 +3051,8 @@
         <f t="shared" si="0"/>
         <v>26.369426751592353</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1568,10 +3063,8 @@
         <f t="shared" si="0"/>
         <v>12.038216560509552</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1582,10 +3075,8 @@
         <f t="shared" si="0"/>
         <v>4.5859872611464967</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -1596,10 +3087,8 @@
         <f t="shared" si="0"/>
         <v>2.8662420382165603</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -1610,8 +3099,6 @@
         <f t="shared" si="0"/>
         <v>19.490445859872612</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -1621,6 +3108,211 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1.55E-4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2.0100000000000001E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2.0699999999999999E-4</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2.6699999999999998E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="6">
+        <v>2.6400000000000002E-4</v>
+      </c>
+      <c r="C23" s="6">
+        <v>3.7200000000000003E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2.03E-4</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2.4000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2.33E-4</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4.3699999999999998E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6">
+        <v>2.9500000000000001E-4</v>
+      </c>
+      <c r="C26" s="6">
+        <v>4.3699999999999998E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.0299999999999999E-4</v>
+      </c>
+      <c r="C27" s="6">
+        <v>7.2600000000000003E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4.1300000000000001E-4</v>
+      </c>
+      <c r="C28" s="6">
+        <v>7.5300000000000001E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="6">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="C29" s="6">
+        <v>9.5000000000000005E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6">
+        <v>5.0900000000000001E-4</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1.2650000000000001E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6">
+        <v>6.5799999999999995E-4</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1.7249999999999999E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B32" s="6">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1.83E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B33" s="6">
+        <v>4.6099999999999998E-4</v>
+      </c>
+      <c r="C33" s="6">
+        <v>2.263E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>2</v>
+      </c>
+      <c r="B34" s="6">
+        <v>5.4900000000000001E-4</v>
+      </c>
+      <c r="C34" s="6">
+        <v>9.3700000000000001E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>3</v>
+      </c>
+      <c r="B35" s="6">
+        <v>6.7100000000000005E-4</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1.6200000000000001E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>3</v>
+      </c>
+      <c r="B36" s="6">
+        <v>8.4199999999999998E-4</v>
+      </c>
+      <c r="C36" s="6">
+        <v>3.7080000000000001E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>4</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1.232E-3</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2.7490000000000001E-4</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:C15">
@@ -1630,6 +3322,7 @@
     <mergeCell ref="A17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>